<commit_message>
Added chart to crimes file
</commit_message>
<xml_diff>
--- a/misc/crime3.xlsx
+++ b/misc/crime3.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\d4d\ddj\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="7275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="7272"/>
   </bookViews>
   <sheets>
     <sheet name="CrimePerGov" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>طوباس</t>
   </si>
@@ -125,11 +120,20 @@
   <si>
     <t>النسبة لكل 1000</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,7 +156,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +199,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -208,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -232,9 +242,6 @@
       <alignment vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
@@ -259,6 +266,19 @@
     <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -274,6 +294,251 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total Crimes per 1000</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.32173955642479363"/>
+          <c:y val="2.0983213429256596E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Crimes per 1000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>CrimePerGov!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v> جنين </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>طوباس</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> طولكرم </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>نابلس</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>قلقيلية</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>سلفيت</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>رام الله والبيرة</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>أريحا والأغوار</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>القدس</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v> بيت لحم </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>الخليل</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CrimePerGov!$B$21:$L$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7.8302834648263131</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.959697893879637</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.981608063812411</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.750870187133843</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.500411850179084</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.496480145708958</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.661342325116804</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.749497655726724</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8592945292002723</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.7868151498451192</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.0073423778255517</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="64893440"/>
+        <c:axId val="166024256"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="64893440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="166024256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="166024256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64893440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>339090</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -319,7 +584,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -352,26 +617,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,23 +652,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -597,30 +828,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P16" sqref="P16"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -664,50 +895,50 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>303565</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>62627</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>178774</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>372621</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>108049</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>69179</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="9">
         <v>338383</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="10">
         <v>50762</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="9">
         <v>411640</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="10">
         <v>210484</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="9">
         <v>684247</v>
       </c>
-      <c r="M2" s="15">
+      <c r="M2" s="14">
         <f>SUM(B2:L2)</f>
         <v>2790331</v>
       </c>
-      <c r="N2" s="16"/>
-    </row>
-    <row r="3" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="15"/>
+    </row>
+    <row r="3" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -751,7 +982,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -795,7 +1026,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -839,7 +1070,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -883,7 +1114,7 @@
         <v>3.24</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -927,7 +1158,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -971,7 +1202,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1015,7 +1246,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1059,7 +1290,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1103,7 +1334,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -1147,7 +1378,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -1191,7 +1422,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -1235,7 +1466,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1279,7 +1510,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1323,7 +1554,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
@@ -1367,7 +1598,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
@@ -1411,7 +1642,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -1455,55 +1686,55 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+    <row r="20" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="12">
         <f>SUM(B3:B19)</f>
         <v>2377</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="12">
         <f t="shared" ref="C20:N20" si="0">SUM(C3:C19)</f>
         <v>749</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="12">
         <f t="shared" si="0"/>
         <v>2142</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="12">
         <f t="shared" si="0"/>
         <v>4006</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="12">
         <f t="shared" si="0"/>
         <v>2107</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="12">
         <f t="shared" si="0"/>
         <v>1833</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="12">
         <f t="shared" si="0"/>
         <v>3946</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="12">
         <f t="shared" si="0"/>
         <v>901</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="12">
         <f t="shared" si="0"/>
         <v>1177</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="12">
         <f t="shared" si="0"/>
         <v>1639</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="12">
         <f t="shared" si="0"/>
         <v>5479</v>
       </c>
-      <c r="M20" s="13">
+      <c r="M20" s="12">
         <f t="shared" si="0"/>
         <v>26356</v>
       </c>
@@ -1512,86 +1743,150 @@
         <v>10.38</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="13">
         <f>(B20/B2)*1000</f>
         <v>7.8302834648263131</v>
       </c>
-      <c r="C21" s="14">
-        <f t="shared" ref="C21:N21" si="1">(C20/C2)*1000</f>
+      <c r="C21" s="13">
+        <f t="shared" ref="C21:M21" si="1">(C20/C2)*1000</f>
         <v>11.959697893879637</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="13">
         <f t="shared" si="1"/>
         <v>11.981608063812411</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="13">
         <f t="shared" si="1"/>
         <v>10.750870187133843</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="13">
         <f t="shared" si="1"/>
         <v>19.500411850179084</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="16">
         <f t="shared" si="1"/>
         <v>26.496480145708958</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="13">
         <f t="shared" si="1"/>
         <v>11.661342325116804</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="13">
         <f t="shared" si="1"/>
         <v>17.749497655726724</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="13">
         <f t="shared" si="1"/>
         <v>2.8592945292002723</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="13">
         <f t="shared" si="1"/>
         <v>7.7868151498451192</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L21" s="13">
         <f t="shared" si="1"/>
         <v>8.0073423778255517</v>
       </c>
-      <c r="M21" s="14">
+      <c r="M21" s="13">
         <f t="shared" si="1"/>
         <v>9.4454743899558871</v>
       </c>
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="1:14" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="21">
+        <f>AVERAGE(B21:L21)</f>
+        <v>12.416694876659518</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="21">
+        <f>_xlfn.STDEV.P(B21:L21)</f>
+        <v>6.2802656848705274</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:14" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="21">
+        <f>MEDIAN(B21:L21)</f>
+        <v>11.661342325116804</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A22:N22"/>
+    <mergeCell ref="A25:N25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="B20:L20" formulaRange="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>